<commit_message>
update task2 visualisation and update Task1.py, generate a jupyternotebook file for furture presentation.
</commit_message>
<xml_diff>
--- a/Task1/EXAMPLE DATA FILE.xlsx
+++ b/Task1/EXAMPLE DATA FILE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunfangyu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunfangyu/Desktop/Charles Data Task/Task1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BB6DA2-57ED-564D-897B-5B4D81D01C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0764A44-1D93-3C4A-834A-8175242AB765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="280" windowWidth="18000" windowHeight="31520" tabRatio="252" xr2:uid="{F7546FD7-615F-444C-99E2-1F435A27CF99}"/>
+    <workbookView xWindow="38400" yWindow="300" windowWidth="18000" windowHeight="31500" tabRatio="252" xr2:uid="{F7546FD7-615F-444C-99E2-1F435A27CF99}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLE CLIENT FILE" sheetId="1" r:id="rId1"/>
@@ -965,12 +965,6 @@
     <t>In the past 12 months, have you seen or heard any advertising for ‘Origin’?</t>
   </si>
   <si>
-    <t>Where did you see or hear advertising for ‘Origin’?</t>
-  </si>
-  <si>
-    <t>Where did you see or hear advertising for ‘Origin’? (Other (please specify))</t>
-  </si>
-  <si>
     <t>Which of the following best describes your current work status?</t>
   </si>
   <si>
@@ -984,6 +978,12 @@
   </si>
   <si>
     <t>Which of the following best describes your household structure? (Other (please specify))</t>
+  </si>
+  <si>
+    <t>Where did you see or hear advertising for 'Origin'? (Other (please specify))</t>
+  </si>
+  <si>
+    <t>Where did you see or hear advertising for 'Origin'?</t>
   </si>
 </sst>
 </file>
@@ -1868,10 +1868,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CFEFDD1-B70F-4E28-A30C-DD955500B403}">
   <dimension ref="A1:X204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="U36" sqref="U36"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1930,25 +1930,25 @@
         <v>308</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>313</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>1</v>

</xml_diff>